<commit_message>
update with plain ratings
</commit_message>
<xml_diff>
--- a/OIA_tupu/tupu_counts_oia.xlsx
+++ b/OIA_tupu/tupu_counts_oia.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="OIAbyband" sheetId="1" state="visible" r:id="rId3"/>
@@ -24,24 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="39">
   <si>
     <t xml:space="preserve">band</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Score1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Score2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Score3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Score4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Score5</t>
   </si>
   <si>
     <t xml:space="preserve">year</t>
@@ -478,28 +463,28 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="2" t="n">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -514,7 +499,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="n">
@@ -535,7 +520,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="n">
@@ -556,7 +541,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="n">
@@ -577,7 +562,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="n">
@@ -598,7 +583,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="n">
@@ -619,7 +604,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="n">
@@ -640,7 +625,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -657,7 +642,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
@@ -674,7 +659,7 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
@@ -693,7 +678,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="n">
@@ -714,7 +699,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="n">
@@ -735,7 +720,7 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="n">
@@ -756,7 +741,7 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -799,39 +784,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="2" t="n">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
@@ -845,10 +830,10 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -864,10 +849,10 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2"/>
@@ -881,10 +866,10 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -898,10 +883,10 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
@@ -923,10 +908,10 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -940,10 +925,10 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -961,10 +946,10 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
@@ -982,10 +967,10 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1007,10 +992,10 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
@@ -1026,10 +1011,10 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
@@ -1049,10 +1034,10 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1066,10 +1051,10 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
@@ -1087,10 +1072,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="2" t="n">
@@ -1114,10 +1099,10 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
@@ -1137,10 +1122,10 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1162,10 +1147,10 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
@@ -1187,10 +1172,10 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1212,10 +1197,10 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1229,10 +1214,10 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
@@ -1252,10 +1237,10 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
@@ -1273,10 +1258,10 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
@@ -1294,10 +1279,10 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
@@ -1319,10 +1304,10 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1336,10 +1321,10 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1357,10 +1342,10 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
@@ -1378,10 +1363,10 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1401,10 +1386,10 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
@@ -1418,10 +1403,10 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -1435,10 +1420,10 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -1452,10 +1437,10 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -1473,10 +1458,10 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="n">
@@ -1500,10 +1485,10 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -1521,10 +1506,10 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -1544,10 +1529,10 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -1565,10 +1550,10 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -1586,10 +1571,10 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -1603,10 +1588,10 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -1622,10 +1607,10 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -1641,10 +1626,10 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -1658,10 +1643,10 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -1675,10 +1660,10 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -1692,10 +1677,10 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -1709,10 +1694,10 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
@@ -1726,10 +1711,10 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -1743,10 +1728,10 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
@@ -1768,10 +1753,10 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
@@ -1785,10 +1770,10 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
@@ -1806,10 +1791,10 @@
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
@@ -1829,10 +1814,10 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4" t="n">
@@ -1856,10 +1841,10 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
@@ -1875,10 +1860,10 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
@@ -1896,10 +1881,10 @@
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -1913,10 +1898,10 @@
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -1936,10 +1921,10 @@
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4" t="n">
@@ -1963,10 +1948,10 @@
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
@@ -1988,10 +1973,10 @@
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
@@ -2013,10 +1998,10 @@
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -2038,10 +2023,10 @@
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
@@ -2063,10 +2048,10 @@
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -2080,10 +2065,10 @@
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
@@ -2103,10 +2088,10 @@
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
@@ -2126,10 +2111,10 @@
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
@@ -2147,10 +2132,10 @@
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
@@ -2172,10 +2157,10 @@
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
@@ -2189,10 +2174,10 @@
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
@@ -2210,10 +2195,10 @@
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -2235,10 +2220,10 @@
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
@@ -2252,10 +2237,10 @@
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
@@ -2273,10 +2258,10 @@
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
@@ -2292,10 +2277,10 @@
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
@@ -2317,10 +2302,10 @@
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
@@ -2338,10 +2323,10 @@
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
@@ -2361,10 +2346,10 @@
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
@@ -2386,10 +2371,10 @@
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
@@ -2409,10 +2394,10 @@
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
@@ -2430,10 +2415,10 @@
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
@@ -2449,10 +2434,10 @@
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
@@ -2490,33 +2475,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="2" t="n">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="n">
@@ -2540,7 +2525,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2554,7 +2539,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
@@ -2572,7 +2557,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2592,7 +2577,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
@@ -2614,7 +2599,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2630,7 +2615,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2650,7 +2635,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
@@ -2664,7 +2649,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2684,7 +2669,7 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="n">
@@ -2708,7 +2693,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
@@ -2728,7 +2713,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2750,7 +2735,7 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -2772,7 +2757,7 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -2794,7 +2779,7 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
@@ -2808,7 +2793,7 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2830,7 +2815,7 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
@@ -2848,7 +2833,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2866,7 +2851,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2888,7 +2873,7 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
@@ -2902,7 +2887,7 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
@@ -2920,7 +2905,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
@@ -2942,7 +2927,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="2" t="n">
@@ -2966,7 +2951,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2982,7 +2967,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3000,7 +2985,7 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
@@ -3014,7 +2999,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3034,7 +3019,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="2" t="n">
@@ -3058,7 +3043,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -3080,7 +3065,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="n">
@@ -3104,7 +3089,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -3126,7 +3111,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -3148,7 +3133,7 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -3164,7 +3149,7 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -3186,7 +3171,7 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -3206,7 +3191,7 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -3366,47 +3351,47 @@
   </sheetPr>
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D76" activeCellId="0" sqref="D76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="2" t="n">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2" t="n">
@@ -3430,10 +3415,10 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -3447,10 +3432,10 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2"/>
@@ -3468,10 +3453,10 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -3491,10 +3476,10 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
@@ -3516,10 +3501,10 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -3535,10 +3520,10 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -3558,10 +3543,10 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
@@ -3575,10 +3560,10 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -3598,10 +3583,10 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="2" t="n">
@@ -3625,10 +3610,10 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
@@ -3648,10 +3633,10 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -3673,10 +3658,10 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
@@ -3698,10 +3683,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
@@ -3723,10 +3708,10 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
@@ -3740,10 +3725,10 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -3765,10 +3750,10 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
@@ -3786,10 +3771,10 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -3807,10 +3792,10 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -3832,10 +3817,10 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
@@ -3849,10 +3834,10 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
@@ -3870,10 +3855,10 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
@@ -3895,10 +3880,10 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="2" t="n">
@@ -3922,10 +3907,10 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -3941,10 +3926,10 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -3962,10 +3947,10 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
@@ -3979,10 +3964,10 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -4002,10 +3987,10 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="2" t="n">
@@ -4029,10 +4014,10 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -4054,10 +4039,10 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="n">
@@ -4081,10 +4066,10 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -4106,10 +4091,10 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -4131,10 +4116,10 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -4150,10 +4135,10 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -4175,10 +4160,10 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -4198,10 +4183,10 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -4361,41 +4346,41 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="2" t="n">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
@@ -4411,7 +4396,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="n">
@@ -4435,7 +4420,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="n">
@@ -4459,7 +4444,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4473,7 +4458,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="n">
@@ -4497,7 +4482,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="n">

</xml_diff>